<commit_message>
Added field responsible by
</commit_message>
<xml_diff>
--- a/docs/Q&A.xlsx
+++ b/docs/Q&A.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Reject ยังต้องทำไหม</t>
   </si>
@@ -90,6 +90,21 @@
   </si>
   <si>
     <t>สภาพแวดล้อมของอุปกรณ์ที่ต้องการตรวจสอบ คืออะไร ต้องการข้อมูลอะไรบ้าง</t>
+  </si>
+  <si>
+    <t>Excise</t>
+  </si>
+  <si>
+    <t>Huawei</t>
+  </si>
+  <si>
+    <t>TOR #</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Responsible by</t>
   </si>
 </sst>
 </file>
@@ -485,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -498,99 +513,136 @@
     <col min="4" max="4" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
+      <c r="C8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>